<commit_message>
Backpropagation neural net initial commit
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Perceptron and backpropagation implemented
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multilayered Net based on backpropagation
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="3">
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -544,13 +544,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5">
@@ -570,10 +570,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -596,13 +596,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oprava chyby v algoritmu zpětné propagace
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.01</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0.99</v>
@@ -550,7 +550,7 @@
         <v>0.01</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -596,10 +596,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.01</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0.99</v>

</xml_diff>

<commit_message>
Final version of notebook
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G2" t="n">
         <v>0.01</v>
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
         <v>0.01</v>

</xml_diff>

<commit_message>
Update backpropagation implementation to use ReLU activation function
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0.01</v>
       </c>
       <c r="H2" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01</v>
+        <v>0.9</v>
       </c>
       <c r="G5" t="n">
-        <v>0.99</v>
+        <v>0.09</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0.01</v>
       </c>
       <c r="H6" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update backpropagation implementation to use Softmax activation function
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -524,7 +524,7 @@
         <v>0.99</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -550,7 +550,7 @@
         <v>0.01</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5">
@@ -576,7 +576,7 @@
         <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Final verison of ReLU a SoftMax
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -495,7 +495,7 @@
         <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0.99</v>
@@ -518,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.49</v>
+        <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>0.51</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -547,10 +547,10 @@
         <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5">
@@ -573,10 +573,10 @@
         <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -599,7 +599,7 @@
         <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0.99</v>

</xml_diff>

<commit_message>
Refactor cross_entropy_loss method in SoftmaxBackPropagation class
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.01</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0.99</v>
@@ -524,7 +524,7 @@
         <v>0.99</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4">
@@ -547,10 +547,10 @@
         <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -576,7 +576,7 @@
         <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -596,10 +596,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.01</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0.99</v>

</xml_diff>

<commit_message>
formating data to float
</commit_message>
<xml_diff>
--- a/diagnosis_output.xlsx
+++ b/diagnosis_output.xlsx
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G2" t="n">
         <v>0.01</v>
@@ -547,7 +547,7 @@
         <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G5" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
         <v>0.01</v>

</xml_diff>